<commit_message>
Add DC^2 Davis County Utah USA
</commit_message>
<xml_diff>
--- a/DCGroups-XLSX/DCGroups-final.xlsx
+++ b/DCGroups-XLSX/DCGroups-final.xlsx
@@ -1,21 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr/>
-  <workbookProtection/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fling\OneDrive\Documents\Github\DCG\DefconGroups\DCGroups-XLSX\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25BA2588-6620-41D2-8923-2CC9B36A7C22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView activeTab="0"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="392">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="405" uniqueCount="395">
   <si>
     <t>ID</t>
   </si>
@@ -1338,24 +1343,33 @@
   <si>
     <t>Sign in to join (https://forum.defcon.org/node/231451)</t>
   </si>
+  <si>
+    <t>DC^2</t>
+  </si>
+  <si>
+    <t>Davis County, Utah USA</t>
+  </si>
+  <si>
+    <t>POC: Zodica
+  - Discord↗ (https://discord.gg/GvjDcCew9Q)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -1371,18 +1385,30 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+  <cellXfs count="3">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -1670,28 +1696,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:F67"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F68"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" topLeftCell="E61" workbookViewId="0">
+      <selection activeCell="E73" sqref="E73"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col customWidth="1" max="1" min="1" width="6"/>
-    <col customWidth="1" max="2" min="2" width="22"/>
-    <col customWidth="1" max="3" min="3" width="40"/>
-    <col customWidth="1" max="4" min="4" width="58"/>
-    <col customWidth="1" max="5" min="5" width="232"/>
-    <col customWidth="1" max="6" min="6" width="56"/>
+    <col min="1" max="1" width="6" customWidth="1"/>
+    <col min="2" max="2" width="22" customWidth="1"/>
+    <col min="3" max="3" width="40" customWidth="1"/>
+    <col min="4" max="4" width="58" customWidth="1"/>
+    <col min="5" max="5" width="232" customWidth="1"/>
+    <col min="6" max="6" width="56" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1711,7 +1733,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
@@ -1731,7 +1753,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>12</v>
       </c>
@@ -1751,7 +1773,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>18</v>
       </c>
@@ -1771,7 +1793,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>24</v>
       </c>
@@ -1791,7 +1813,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>30</v>
       </c>
@@ -1811,7 +1833,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>36</v>
       </c>
@@ -1831,7 +1853,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>42</v>
       </c>
@@ -1851,7 +1873,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>48</v>
       </c>
@@ -1871,7 +1893,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>54</v>
       </c>
@@ -1891,7 +1913,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>60</v>
       </c>
@@ -1911,7 +1933,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>65</v>
       </c>
@@ -1931,7 +1953,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>71</v>
       </c>
@@ -1951,7 +1973,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>77</v>
       </c>
@@ -1971,7 +1993,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>83</v>
       </c>
@@ -1991,7 +2013,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>89</v>
       </c>
@@ -2011,7 +2033,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>95</v>
       </c>
@@ -2031,7 +2053,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>101</v>
       </c>
@@ -2051,7 +2073,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>107</v>
       </c>
@@ -2071,7 +2093,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>112</v>
       </c>
@@ -2091,7 +2113,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>118</v>
       </c>
@@ -2111,7 +2133,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>124</v>
       </c>
@@ -2131,7 +2153,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>129</v>
       </c>
@@ -2151,7 +2173,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>135</v>
       </c>
@@ -2171,7 +2193,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="25" spans="1:6">
+    <row r="25" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>141</v>
       </c>
@@ -2191,7 +2213,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>147</v>
       </c>
@@ -2211,7 +2233,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="27" spans="1:6">
+    <row r="27" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>153</v>
       </c>
@@ -2231,7 +2253,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="28" spans="1:6">
+    <row r="28" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>158</v>
       </c>
@@ -2251,7 +2273,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="29" spans="1:6">
+    <row r="29" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>163</v>
       </c>
@@ -2271,7 +2293,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="30" spans="1:6">
+    <row r="30" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>169</v>
       </c>
@@ -2291,7 +2313,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="31" spans="1:6">
+    <row r="31" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>175</v>
       </c>
@@ -2311,7 +2333,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="32" spans="1:6">
+    <row r="32" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>181</v>
       </c>
@@ -2331,7 +2353,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="33" spans="1:6">
+    <row r="33" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>187</v>
       </c>
@@ -2351,7 +2373,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="34" spans="1:6">
+    <row r="34" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>193</v>
       </c>
@@ -2371,7 +2393,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="35" spans="1:6">
+    <row r="35" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>199</v>
       </c>
@@ -2391,7 +2413,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="36" spans="1:6">
+    <row r="36" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>204</v>
       </c>
@@ -2411,7 +2433,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="37" spans="1:6">
+    <row r="37" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>210</v>
       </c>
@@ -2431,7 +2453,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="38" spans="1:6">
+    <row r="38" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>216</v>
       </c>
@@ -2451,7 +2473,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="39" spans="1:6">
+    <row r="39" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>221</v>
       </c>
@@ -2471,7 +2493,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="40" spans="1:6">
+    <row r="40" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>226</v>
       </c>
@@ -2491,7 +2513,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="41" spans="1:6">
+    <row r="41" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>232</v>
       </c>
@@ -2511,7 +2533,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="42" spans="1:6">
+    <row r="42" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>238</v>
       </c>
@@ -2531,7 +2553,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="43" spans="1:6">
+    <row r="43" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>244</v>
       </c>
@@ -2551,7 +2573,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="44" spans="1:6">
+    <row r="44" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>250</v>
       </c>
@@ -2571,7 +2593,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="45" spans="1:6">
+    <row r="45" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>256</v>
       </c>
@@ -2591,7 +2613,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="46" spans="1:6">
+    <row r="46" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>262</v>
       </c>
@@ -2611,7 +2633,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="47" spans="1:6">
+    <row r="47" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>268</v>
       </c>
@@ -2631,7 +2653,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="48" spans="1:6">
+    <row r="48" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>274</v>
       </c>
@@ -2651,7 +2673,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="49" spans="1:6">
+    <row r="49" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>279</v>
       </c>
@@ -2671,7 +2693,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="50" spans="1:6">
+    <row r="50" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>285</v>
       </c>
@@ -2691,7 +2713,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="51" spans="1:6">
+    <row r="51" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>291</v>
       </c>
@@ -2711,7 +2733,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="52" spans="1:6">
+    <row r="52" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>297</v>
       </c>
@@ -2731,7 +2753,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="53" spans="1:6">
+    <row r="53" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>303</v>
       </c>
@@ -2751,7 +2773,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="54" spans="1:6">
+    <row r="54" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>309</v>
       </c>
@@ -2771,7 +2793,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="55" spans="1:6">
+    <row r="55" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>315</v>
       </c>
@@ -2791,7 +2813,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="56" spans="1:6">
+    <row r="56" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>321</v>
       </c>
@@ -2811,7 +2833,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="57" spans="1:6">
+    <row r="57" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>327</v>
       </c>
@@ -2831,7 +2853,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="58" spans="1:6">
+    <row r="58" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>333</v>
       </c>
@@ -2851,7 +2873,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="59" spans="1:6">
+    <row r="59" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>339</v>
       </c>
@@ -2871,7 +2893,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="60" spans="1:6">
+    <row r="60" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>345</v>
       </c>
@@ -2891,7 +2913,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="61" spans="1:6">
+    <row r="61" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>350</v>
       </c>
@@ -2911,7 +2933,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="62" spans="1:6">
+    <row r="62" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>356</v>
       </c>
@@ -2931,7 +2953,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="63" spans="1:6">
+    <row r="63" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>362</v>
       </c>
@@ -2951,7 +2973,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="64" spans="1:6">
+    <row r="64" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>368</v>
       </c>
@@ -2971,7 +2993,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="65" spans="1:6">
+    <row r="65" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>374</v>
       </c>
@@ -2991,7 +3013,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="66" spans="1:6">
+    <row r="66" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>380</v>
       </c>
@@ -3011,7 +3033,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="67" spans="1:6">
+    <row r="67" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>386</v>
       </c>
@@ -3031,7 +3053,21 @@
         <v>391</v>
       </c>
     </row>
+    <row r="68" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A68" s="2">
+        <v>66</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>392</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>393</v>
+      </c>
+      <c r="E68" s="1" t="s">
+        <v>394</v>
+      </c>
+    </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>